<commit_message>
Update rules to v2
</commit_message>
<xml_diff>
--- a/Words before and after traits_v2.xlsx
+++ b/Words before and after traits_v2.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vuw-my.sharepoint.com/personal/ciarleri_staff_vuw_ac_nz/Documents/Desktop/Insular assembly rules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/simone_monaco_polito_it/Documents/Documenti/PoliTO/NewZeland/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="928" documentId="11_F25DC773A252ABDACC10485469DC60605ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13FCFD46-C27C-47CE-B44E-C0FC674CED7E}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{B96F9A42-91C1-41E8-9842-B794338A7FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AF363CB-5CD3-4C5A-8357-B32EDC728E06}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Traits" sheetId="2" r:id="rId1"/>
     <sheet name="Words" sheetId="1" r:id="rId2"/>
-    <sheet name="Flower searches" sheetId="3" r:id="rId3"/>
-    <sheet name="IF" sheetId="4" r:id="rId4"/>
+    <sheet name="Words_legacy" sheetId="5" r:id="rId3"/>
+    <sheet name="Flower searches" sheetId="3" r:id="rId4"/>
+    <sheet name="IF" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,8 +28,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={2D23C5D7-737E-44B9-8C65-12C2EDD86C5F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{2D23C5D7-737E-44B9-8C65-12C2EDD86C5F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    petiolules è una keyword che può andare qui?</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="445">
   <si>
     <t>Stature</t>
   </si>
@@ -1327,13 +1346,49 @@
   </si>
   <si>
     <t>Ray floret size</t>
+  </si>
+  <si>
+    <t>Pistillate</t>
+  </si>
+  <si>
+    <t>Staminate</t>
+  </si>
+  <si>
+    <t>Tubes</t>
+  </si>
+  <si>
+    <t>Floret</t>
+  </si>
+  <si>
+    <t>Florets</t>
+  </si>
+  <si>
+    <t>Sparire long</t>
+  </si>
+  <si>
+    <t>Togliere ; prima di ogni misura</t>
+  </si>
+  <si>
+    <t>Stygma</t>
+  </si>
+  <si>
+    <t>Culms</t>
+  </si>
+  <si>
+    <t>Tall</t>
+  </si>
+  <si>
+    <t>Sessil</t>
+  </si>
+  <si>
+    <t>Ray</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1354,6 +1409,28 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="7"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1388,7 +1465,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1397,26 +1474,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1426,19 +1487,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1454,6 +1518,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Simone  Monaco" id="{3F739B71-14D4-4447-80E8-60C5A1936E17}" userId="S::simone.monaco@polito.it::681e8622-bdd4-4909-b697-8175fe219ecb" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1717,6 +1787,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D2" dT="2023-11-09T16:53:19.39" personId="{3F739B71-14D4-4447-80E8-60C5A1936E17}" id="{2D23C5D7-737E-44B9-8C65-12C2EDD86C5F}">
+    <text>petiolules è una keyword che può andare qui?</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44F8C65-5ACD-4DAE-A8C7-72B9B0DF9C11}">
   <dimension ref="A1:B26"/>
@@ -1725,179 +1803,179 @@
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="12"/>
+      <c r="B7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="12"/>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="12"/>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="12"/>
+      <c r="B10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="12"/>
+      <c r="B11" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="12"/>
+      <c r="B12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
-      <c r="B13" s="4" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="12"/>
+      <c r="B14" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="4" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="12"/>
+      <c r="B15" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
+      <c r="B16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="12"/>
+      <c r="B17" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="12"/>
+      <c r="B18" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
+      <c r="B19" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
-      <c r="B20" s="4" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="12"/>
+      <c r="B20" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="18"/>
-      <c r="B22" s="4" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
+      <c r="B22" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="12"/>
+      <c r="B23" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="17"/>
-      <c r="B25" s="4" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
+      <c r="B25" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1910,147 +1988,1676 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.88671875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13" style="3" customWidth="1"/>
+    <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.44140625" style="3" customWidth="1"/>
+    <col min="19" max="20" width="12" style="3" customWidth="1"/>
+    <col min="21" max="21" width="9.5546875" style="3" customWidth="1"/>
+    <col min="22" max="22" width="16.33203125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="12" style="3" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="14.109375" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>369</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z2" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="R3" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="S3" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="T3" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="U3" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="V3" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>444</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>331</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="M4" s="15" t="s">
+        <v>443</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="P4" s="15" t="s">
+        <v>325</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>333</v>
+      </c>
+      <c r="R4" s="15" t="s">
+        <v>335</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>327</v>
+      </c>
+      <c r="T4" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="U4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="W4" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="X4" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="Y4" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z4" s="5" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="V5" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="W5" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="X5" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="Z5" s="5" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
+        <v>299</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="N6" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>358</v>
+      </c>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15" t="s">
+        <v>252</v>
+      </c>
+      <c r="V6" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="Z6" s="5" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15" t="s">
+        <v>440</v>
+      </c>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="X7" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="Z7" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15"/>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z8" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15"/>
+      <c r="V10" s="15" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15" t="s">
+        <v>340</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A12" s="15"/>
+      <c r="B12" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="15" t="s">
+        <v>376</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A13" s="15"/>
+      <c r="B13" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15"/>
+      <c r="V13" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" s="15"/>
+      <c r="B14" s="15" t="s">
+        <v>364</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="F14" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15"/>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15"/>
+      <c r="V14" s="15" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" s="15"/>
+      <c r="B15" s="15" t="s">
+        <v>365</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15" t="s">
+        <v>441</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15"/>
+      <c r="V15" s="15" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" s="15"/>
+      <c r="B16" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>337</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
+      <c r="M17" s="15"/>
+      <c r="N17" s="15"/>
+      <c r="O17" s="15"/>
+      <c r="P17" s="15"/>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15"/>
+      <c r="S17" s="15"/>
+      <c r="T17" s="15"/>
+      <c r="U17" s="15"/>
+      <c r="V17" s="15"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="15" t="s">
+        <v>338</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="15"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="15"/>
+      <c r="O18" s="15"/>
+      <c r="P18" s="15"/>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15"/>
+      <c r="S18" s="15"/>
+      <c r="T18" s="15"/>
+      <c r="U18" s="15"/>
+      <c r="V18" s="15"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15" t="s">
+        <v>343</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="15" t="s">
+        <v>345</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="15"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
+      <c r="S21" s="15"/>
+      <c r="T21" s="15"/>
+      <c r="U21" s="15"/>
+      <c r="V21" s="15"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="15"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
+      <c r="S22" s="15"/>
+      <c r="T22" s="15"/>
+      <c r="U22" s="15"/>
+      <c r="V22" s="15"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15" t="s">
+        <v>341</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="15"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
+      <c r="S23" s="15"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15" t="s">
+        <v>342</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="15"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
+      <c r="S24" s="15"/>
+      <c r="T24" s="15"/>
+      <c r="U24" s="15"/>
+      <c r="V24" s="15"/>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15" t="s">
+        <v>347</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
+      <c r="S25" s="15"/>
+      <c r="T25" s="15"/>
+      <c r="U25" s="15"/>
+      <c r="V25" s="15"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15" t="s">
+        <v>349</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15" t="s">
+        <v>350</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="U34" s="2"/>
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="K35" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V35" s="2"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J36" s="2"/>
+      <c r="K36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2"/>
+      <c r="R36" s="2"/>
+      <c r="S36" s="2"/>
+      <c r="T36" s="2"/>
+      <c r="U36" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="V36" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="R37" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="S37" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="T37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="U37" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="V37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="W37" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="X37" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>422</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="S39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="T39" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="U39" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="V39" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="W39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X39" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="N40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="O40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="T40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="O41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="S41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="T41" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="V41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W41" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="X41" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B42" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B43" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="V43" s="3" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B44" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V44" s="5" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B45" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="B46" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51DEC615-39EB-4857-AAA5-ED84157C4825}">
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5703125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.28515625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.5546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.33203125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" style="3" customWidth="1"/>
     <col min="15" max="15" width="13" style="3" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="12.42578125" style="3" customWidth="1"/>
+    <col min="17" max="18" width="12.44140625" style="3" customWidth="1"/>
     <col min="19" max="21" width="12" style="3" customWidth="1"/>
-    <col min="22" max="22" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" style="3" customWidth="1"/>
-    <col min="24" max="24" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.140625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="14.140625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="14.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="14.109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="N2" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="V2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="8" t="s">
         <v>359</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="8" t="s">
         <v>369</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="8" t="s">
         <v>375</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="8" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -2099,16 +3706,16 @@
       <c r="P3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q3" s="7" t="s">
+      <c r="Q3" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="3" t="s">
         <v>119</v>
       </c>
       <c r="U3" s="3" t="s">
@@ -2117,20 +3724,20 @@
       <c r="V3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="W3" s="10" t="s">
+      <c r="W3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="10" t="s">
+      <c r="X3" s="5" t="s">
         <v>370</v>
       </c>
-      <c r="Y3" s="10" t="s">
+      <c r="Y3" s="5" t="s">
         <v>310</v>
       </c>
-      <c r="Z3" s="10" t="s">
+      <c r="Z3" s="5" t="s">
         <v>394</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>36</v>
       </c>
@@ -2197,20 +3804,20 @@
       <c r="V4" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" s="5" t="s">
         <v>346</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="X4" s="5" t="s">
         <v>371</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" s="5" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>53</v>
       </c>
@@ -2229,10 +3836,10 @@
       <c r="F5" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="5" t="s">
         <v>329</v>
       </c>
       <c r="I5" s="3" t="s">
@@ -2253,19 +3860,19 @@
       <c r="N5" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="5" t="s">
         <v>324</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="5" t="s">
         <v>325</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="5" t="s">
         <v>333</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="5" t="s">
         <v>328</v>
       </c>
       <c r="T5" s="3" t="s">
@@ -2277,17 +3884,17 @@
       <c r="V5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="5" t="s">
         <v>385</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="5" t="s">
         <v>398</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="Z5" s="5" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>73</v>
       </c>
@@ -2303,10 +3910,10 @@
       <c r="E6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="5" t="s">
         <v>330</v>
       </c>
       <c r="I6" s="3" t="s">
@@ -2318,28 +3925,28 @@
       <c r="K6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="O6" s="10" t="s">
+      <c r="O6" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="S6" s="10" t="s">
+      <c r="S6" s="5" t="s">
         <v>327</v>
       </c>
       <c r="T6" s="3" t="s">
@@ -2351,17 +3958,17 @@
       <c r="V6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="W6" s="10" t="s">
+      <c r="W6" s="5" t="s">
         <v>386</v>
       </c>
-      <c r="X6" s="10" t="s">
+      <c r="X6" s="5" t="s">
         <v>399</v>
       </c>
-      <c r="Z6" s="10" t="s">
+      <c r="Z6" s="5" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>86</v>
       </c>
@@ -2371,44 +3978,44 @@
       <c r="C7" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="3" t="s">
         <v>299</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="5" t="s">
         <v>361</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="O7" s="10" t="s">
+      <c r="O7" s="5" t="s">
         <v>357</v>
       </c>
-      <c r="U7" s="10" t="s">
+      <c r="U7" s="5" t="s">
         <v>353</v>
       </c>
       <c r="V7" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>87</v>
       </c>
@@ -2425,16 +4032,16 @@
       <c r="I8" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="5" t="s">
         <v>373</v>
       </c>
-      <c r="K8" s="12" t="s">
+      <c r="K8" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="O8" s="10" t="s">
+      <c r="O8" s="5" t="s">
         <v>358</v>
       </c>
       <c r="U8" s="3" t="s">
@@ -2444,7 +4051,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>88</v>
       </c>
@@ -2461,20 +4068,20 @@
       <c r="I9" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="5" t="s">
         <v>374</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="5" t="s">
         <v>252</v>
       </c>
       <c r="U9" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="V9" s="10" t="s">
+      <c r="V9" s="5" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>277</v>
       </c>
@@ -2482,24 +4089,23 @@
       <c r="C10" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="6" t="s">
         <v>115</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="9"/>
       <c r="I10" s="3" t="s">
         <v>265</v>
       </c>
       <c r="U10" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="V10" s="10" t="s">
+      <c r="V10" s="5" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>278</v>
       </c>
@@ -2519,11 +4125,11 @@
       <c r="U11" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="V11" s="10" t="s">
+      <c r="V11" s="5" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>279</v>
       </c>
@@ -2540,11 +4146,11 @@
       <c r="U12" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="V12" s="10" t="s">
+      <c r="V12" s="5" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>280</v>
       </c>
@@ -2561,33 +4167,33 @@
       <c r="U13" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="V13" s="10" t="s">
+      <c r="V13" s="5" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>415</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="5" t="s">
         <v>382</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="V14" s="10" t="s">
+      <c r="V14" s="5" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
         <v>411</v>
       </c>
       <c r="B15" s="3"/>
@@ -2597,352 +4203,348 @@
       <c r="D15" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="5" t="s">
         <v>383</v>
       </c>
       <c r="U15" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="V15" s="10" t="s">
+      <c r="V15" s="5" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
         <v>412</v>
       </c>
       <c r="B16" s="3"/>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="5" t="s">
         <v>376</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="5" t="s">
         <v>387</v>
       </c>
-      <c r="U16" s="7" t="s">
+      <c r="U16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="V16" s="10" t="s">
+      <c r="V16" s="5" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>413</v>
       </c>
       <c r="B17" s="3"/>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="5" t="s">
         <v>377</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="5" t="s">
         <v>388</v>
       </c>
-      <c r="U17" s="11" t="s">
+      <c r="U17" s="5" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
         <v>414</v>
       </c>
       <c r="B18" s="3"/>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="U18" s="11" t="s">
+      <c r="U18" s="5" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
         <v>416</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="U19" s="11" t="s">
+      <c r="U19" s="5" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="5" t="s">
         <v>405</v>
       </c>
-      <c r="U20" s="11" t="s">
+      <c r="U20" s="5" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="5" t="s">
         <v>404</v>
       </c>
-      <c r="U21" s="11" t="s">
+      <c r="U21" s="5" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
-      <c r="D22" s="16" t="s">
+      <c r="D22" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="5" t="s">
         <v>406</v>
       </c>
-      <c r="U22" s="10" t="s">
+      <c r="U22" s="5" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
-      <c r="D23" s="10" t="s">
+      <c r="D23" s="5" t="s">
         <v>317</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E23" s="5" t="s">
         <v>407</v>
       </c>
-      <c r="U23" s="10" t="s">
+      <c r="U23" s="5" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="5" t="s">
         <v>418</v>
       </c>
-      <c r="U24" s="10" t="s">
+      <c r="U24" s="5" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="5" t="s">
         <v>419</v>
       </c>
-      <c r="U25" s="10" t="s">
+      <c r="U25" s="5" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="5" t="s">
         <v>320</v>
       </c>
-      <c r="U26" s="10" t="s">
+      <c r="U26" s="5" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="5" t="s">
         <v>321</v>
       </c>
-      <c r="U27" s="10" t="s">
+      <c r="U27" s="5" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="U28" s="10" t="s">
+      <c r="U28" s="5" t="s">
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
-      <c r="U29" s="10" t="s">
+      <c r="U29" s="5" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
-      <c r="U30" s="10" t="s">
+      <c r="U30" s="5" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="U31" s="10" t="s">
+      <c r="U31" s="5" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
-      <c r="U32" s="9"/>
-    </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="U33" s="9"/>
-    </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="U34" s="9"/>
-    </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
-      <c r="U35" s="9"/>
-    </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
-      <c r="N36" s="19"/>
-      <c r="O36" s="19"/>
-      <c r="P36" s="19"/>
-      <c r="Q36" s="19"/>
-      <c r="R36" s="19"/>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19"/>
-      <c r="U36" s="19"/>
-      <c r="V36" s="19"/>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+      <c r="Q36" s="13"/>
+      <c r="R36" s="13"/>
+      <c r="S36" s="13"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="13"/>
+      <c r="V36" s="13"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="G37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I37" s="5" t="s">
+      <c r="I37" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L37" s="5" t="s">
+      <c r="L37" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="M37" s="5" t="s">
+      <c r="M37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N37" s="5" t="s">
+      <c r="N37" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="O37" s="5" t="s">
+      <c r="O37" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="P37" s="5" t="s">
+      <c r="P37" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q37" s="5" t="s">
+      <c r="Q37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="R37" s="5" t="s">
+      <c r="R37" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="S37" s="5" t="s">
+      <c r="S37" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="T37" s="5" t="s">
+      <c r="T37" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="U37" s="5" t="s">
+      <c r="U37" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V37" s="5" t="s">
+      <c r="V37" s="2" t="s">
         <v>19</v>
       </c>
       <c r="W37" s="3" t="s">
@@ -2952,7 +4554,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>46</v>
       </c>
@@ -3026,7 +4628,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>75</v>
       </c>
@@ -3100,7 +4702,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>154</v>
       </c>
@@ -3174,7 +4776,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>155</v>
       </c>
@@ -3248,8 +4850,8 @@
         <v>372</v>
       </c>
     </row>
-    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A42" s="5" t="s">
         <v>422</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -3274,7 +4876,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -3294,7 +4896,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D44" s="3" t="s">
         <v>46</v>
       </c>
@@ -3308,11 +4910,11 @@
         <v>92</v>
       </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="D45" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E45" s="10" t="s">
+      <c r="E45" s="5" t="s">
         <v>427</v>
       </c>
       <c r="U45" s="3" t="s">
@@ -3322,22 +4924,22 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="V46" s="3" t="s">
         <v>100</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A1:V1"/>
     <mergeCell ref="A36:V36"/>
-    <mergeCell ref="A1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F3B4F2-2D7E-48BD-B45D-E85DB15729D5}">
   <dimension ref="A1:D111"/>
   <sheetViews>
@@ -3345,15 +4947,15 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>128</v>
       </c>
@@ -3367,7 +4969,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>258</v>
       </c>
@@ -3381,7 +4983,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>131</v>
@@ -3393,7 +4995,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>132</v>
@@ -3402,7 +5004,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>133</v>
@@ -3411,7 +5013,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
         <v>134</v>
@@ -3420,631 +5022,631 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2"/>
       <c r="B14" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="2"/>
       <c r="B19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="2"/>
       <c r="B20" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="2"/>
       <c r="B21" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="2"/>
       <c r="B35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="2"/>
       <c r="B36" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="2"/>
       <c r="B37" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="2"/>
       <c r="B38" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="2"/>
       <c r="B41" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="2"/>
       <c r="B43" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="2"/>
       <c r="B45" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="2"/>
       <c r="B46" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="2"/>
       <c r="B47" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="2"/>
       <c r="B48" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="2"/>
       <c r="B49" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2"/>
       <c r="B52" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="2"/>
       <c r="B53" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="2"/>
       <c r="B54" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="2"/>
       <c r="B55" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="2"/>
       <c r="B65" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
       <c r="B66" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
       <c r="B67" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
       <c r="B68" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
       <c r="B69" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" s="2"/>
       <c r="B70" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" s="2"/>
       <c r="B81" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" s="2"/>
       <c r="B82" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" s="2"/>
       <c r="B83" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" s="2"/>
       <c r="B84" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" s="2"/>
       <c r="B85" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" s="2"/>
       <c r="B86" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" s="2"/>
       <c r="B87" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="2"/>
       <c r="B93" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="2"/>
       <c r="B94" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="2"/>
       <c r="B95" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="2"/>
       <c r="B96" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="2"/>
       <c r="B97" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="2"/>
       <c r="B98" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="2"/>
-      <c r="B99" s="4" t="s">
+      <c r="B99" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="2"/>
       <c r="B100" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="2"/>
       <c r="B101" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="2"/>
       <c r="B102" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="2"/>
       <c r="B103" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="2"/>
       <c r="B104" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="2"/>
       <c r="B105" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="2"/>
       <c r="B106" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="2"/>
       <c r="B107" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="2"/>
       <c r="B108" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="2"/>
       <c r="B109" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="2"/>
       <c r="B110" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="2"/>
       <c r="B111" s="1"/>
     </row>
@@ -4053,29 +5655,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DA1169-2C93-47A0-96CD-8055F1566B0F}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="139" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="123" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="2" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>303</v>
       </c>
@@ -4083,7 +5685,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>304</v>
       </c>
@@ -4091,7 +5693,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>305</v>
       </c>
@@ -4099,7 +5701,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>306</v>
       </c>
@@ -4107,7 +5709,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>272</v>
       </c>
@@ -4115,7 +5717,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>276</v>
       </c>
@@ -4123,7 +5725,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>282</v>
       </c>
@@ -4131,7 +5733,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>289</v>
       </c>
@@ -4139,7 +5741,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>287</v>
       </c>
@@ -4147,7 +5749,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>288</v>
       </c>
@@ -4155,7 +5757,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>300</v>
       </c>
@@ -4163,7 +5765,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -4171,145 +5773,153 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
         <v>351</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="7" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
         <v>355</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="7" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
         <v>356</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="7" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="7" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
         <v>378</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="7" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="19" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="7" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>408</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="7" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="21" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="22" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="15" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="15" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="B25" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B29" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B31" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="10" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="10" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="10" t="s">
         <v>426</v>
       </c>
     </row>

</xml_diff>